<commit_message>
This is commit for DDTest
</commit_message>
<xml_diff>
--- a/testData/Userdata.xlsx
+++ b/testData/Userdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavan\restAssuredTraining\PetStoreAutomation\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\API_Testing_PetStoreAutomation\PetStoreAutomation\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E65099-367B-4043-98C2-1CDC1656E877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2990CE-3331-46DB-9AC7-AF18B88C0D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3146" windowWidth="22303" windowHeight="11974" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,21 +460,21 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.23046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.15234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>1010</v>
       </c>
@@ -520,7 +520,7 @@
         <v>1234567897</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>1020</v>
       </c>
@@ -543,7 +543,7 @@
         <v>1234567897</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>1030</v>
       </c>

</xml_diff>